<commit_message>
added sacramento plus SCC presentation
</commit_message>
<xml_diff>
--- a/santa_clara_county/CFR_LTCF.xlsx
+++ b/santa_clara_county/CFR_LTCF.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\stk\Documents\GitHub\covid\santa_clara_county\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90D871D0-A5F7-4D5C-9C5E-97F1F016E721}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53E3F3D1-12DD-41D9-9AFF-6B24A8B722D9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="3" activeTab="5" xr2:uid="{92AC6A02-C79A-4134-BBFB-5A0657F9F650}"/>
   </bookViews>
@@ -22,7 +22,7 @@
   </sheets>
   <calcPr calcId="191029"/>
   <pivotCaches>
-    <pivotCache cacheId="41" r:id="rId7"/>
+    <pivotCache cacheId="0" r:id="rId7"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="42">
   <si>
     <t>New_cases</t>
   </si>
@@ -178,6 +178,9 @@
   <si>
     <t>Q2 21</t>
   </si>
+  <si>
+    <t>For plot:</t>
+  </si>
 </sst>
 </file>
 
@@ -186,7 +189,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="m/d/yy;@"/>
   </numFmts>
-  <fonts count="19" x14ac:knownFonts="1">
+  <fonts count="20" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -325,6 +328,13 @@
       <b/>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -686,7 +696,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="16" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -708,6 +718,8 @@
       <alignment horizontal="left" indent="2"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -857,7 +869,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>'pivot by qtr w plot'!$A$16:$A$21</c:f>
+              <c:f>'pivot by qtr w plot'!$G$19:$G$24</c:f>
               <c:strCache>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
@@ -883,7 +895,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'pivot by qtr w plot'!$B$16:$B$21</c:f>
+              <c:f>'pivot by qtr w plot'!$H$19:$H$24</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
@@ -4170,7 +4182,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{3912446F-DA69-460E-A455-88B8521F7EDA}" name="PivotTable12" cacheId="41" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{3912446F-DA69-460E-A455-88B8521F7EDA}" name="PivotTable12" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A3:C27" firstHeaderRow="0" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="6">
     <pivotField axis="axisRow" numFmtId="164" showAll="0">
@@ -4733,8 +4745,8 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{F25E3E1A-821A-4C97-B531-A1F853788CC3}" name="PivotTable12" cacheId="41" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
-  <location ref="A3:C12" firstHeaderRow="0" firstDataRow="1" firstDataCol="1"/>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{F25E3E1A-821A-4C97-B531-A1F853788CC3}" name="PivotTable12" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+  <location ref="A3:C27" firstHeaderRow="0" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="6">
     <pivotField axis="axisRow" numFmtId="164" showAll="0">
       <items count="406">
@@ -5170,10 +5182,10 @@
     <pivotField axis="axisRow" showAll="0">
       <items count="7">
         <item sd="0" x="0"/>
-        <item sd="0" x="1"/>
-        <item sd="0" x="2"/>
-        <item sd="0" x="3"/>
-        <item sd="0" x="4"/>
+        <item x="1"/>
+        <item x="2"/>
+        <item x="3"/>
+        <item x="4"/>
         <item sd="0" x="5"/>
         <item t="default"/>
       </items>
@@ -5194,21 +5206,54 @@
     <field x="3"/>
     <field x="0"/>
   </rowFields>
-  <rowItems count="9">
+  <rowItems count="24">
     <i>
       <x v="1"/>
     </i>
     <i r="1">
       <x v="1"/>
     </i>
+    <i r="2">
+      <x v="2"/>
+    </i>
+    <i r="2">
+      <x v="3"/>
+    </i>
     <i r="1">
       <x v="2"/>
+    </i>
+    <i r="2">
+      <x v="4"/>
+    </i>
+    <i r="2">
+      <x v="5"/>
+    </i>
+    <i r="2">
+      <x v="6"/>
     </i>
     <i r="1">
       <x v="3"/>
     </i>
+    <i r="2">
+      <x v="7"/>
+    </i>
+    <i r="2">
+      <x v="8"/>
+    </i>
+    <i r="2">
+      <x v="9"/>
+    </i>
     <i r="1">
       <x v="4"/>
+    </i>
+    <i r="2">
+      <x v="10"/>
+    </i>
+    <i r="2">
+      <x v="11"/>
+    </i>
+    <i r="2">
+      <x v="12"/>
     </i>
     <i>
       <x v="2"/>
@@ -5216,8 +5261,20 @@
     <i r="1">
       <x v="1"/>
     </i>
+    <i r="2">
+      <x v="1"/>
+    </i>
+    <i r="2">
+      <x v="2"/>
+    </i>
+    <i r="2">
+      <x v="3"/>
+    </i>
     <i r="1">
       <x v="2"/>
+    </i>
+    <i r="2">
+      <x v="4"/>
     </i>
     <i t="grand">
       <x/>
@@ -33458,10 +33515,10 @@
       <c r="A4" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="B4" s="10">
+      <c r="B4">
         <v>5349</v>
       </c>
-      <c r="C4" s="10">
+      <c r="C4">
         <v>574</v>
       </c>
       <c r="E4">
@@ -33473,10 +33530,10 @@
       <c r="A5" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="B5" s="10">
+      <c r="B5">
         <v>101</v>
       </c>
-      <c r="C5" s="10">
+      <c r="C5">
         <v>13</v>
       </c>
       <c r="E5">
@@ -33488,10 +33545,10 @@
       <c r="A6" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="B6" s="10">
-        <v>1</v>
-      </c>
-      <c r="C6" s="10">
+      <c r="B6">
+        <v>1</v>
+      </c>
+      <c r="C6">
         <v>0</v>
       </c>
       <c r="E6">
@@ -33503,10 +33560,10 @@
       <c r="A7" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="B7" s="10">
+      <c r="B7">
         <v>100</v>
       </c>
-      <c r="C7" s="10">
+      <c r="C7">
         <v>13</v>
       </c>
       <c r="E7">
@@ -33518,10 +33575,10 @@
       <c r="A8" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="B8" s="10">
+      <c r="B8">
         <v>779</v>
       </c>
-      <c r="C8" s="10">
+      <c r="C8">
         <v>62</v>
       </c>
       <c r="E8">
@@ -33533,10 +33590,10 @@
       <c r="A9" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="B9" s="10">
+      <c r="B9">
         <v>439</v>
       </c>
-      <c r="C9" s="10">
+      <c r="C9">
         <v>41</v>
       </c>
       <c r="E9">
@@ -33548,10 +33605,10 @@
       <c r="A10" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="B10" s="10">
+      <c r="B10">
         <v>113</v>
       </c>
-      <c r="C10" s="10">
+      <c r="C10">
         <v>9</v>
       </c>
       <c r="E10">
@@ -33563,10 +33620,10 @@
       <c r="A11" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="B11" s="10">
+      <c r="B11">
         <v>227</v>
       </c>
-      <c r="C11" s="10">
+      <c r="C11">
         <v>12</v>
       </c>
       <c r="E11">
@@ -33578,10 +33635,10 @@
       <c r="A12" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="B12" s="10">
+      <c r="B12">
         <v>720</v>
       </c>
-      <c r="C12" s="10">
+      <c r="C12">
         <v>61</v>
       </c>
       <c r="E12">
@@ -33593,10 +33650,10 @@
       <c r="A13" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="B13" s="10">
+      <c r="B13">
         <v>254</v>
       </c>
-      <c r="C13" s="10">
+      <c r="C13">
         <v>11</v>
       </c>
       <c r="E13">
@@ -33608,10 +33665,10 @@
       <c r="A14" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="B14" s="10">
+      <c r="B14">
         <v>265</v>
       </c>
-      <c r="C14" s="10">
+      <c r="C14">
         <v>31</v>
       </c>
       <c r="E14">
@@ -33623,10 +33680,10 @@
       <c r="A15" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="B15" s="10">
+      <c r="B15">
         <v>201</v>
       </c>
-      <c r="C15" s="10">
+      <c r="C15">
         <v>19</v>
       </c>
       <c r="E15">
@@ -33638,10 +33695,10 @@
       <c r="A16" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="B16" s="10">
+      <c r="B16">
         <v>3749</v>
       </c>
-      <c r="C16" s="10">
+      <c r="C16">
         <v>438</v>
       </c>
       <c r="E16">
@@ -33653,10 +33710,10 @@
       <c r="A17" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="B17" s="10">
+      <c r="B17">
         <v>244</v>
       </c>
-      <c r="C17" s="10">
+      <c r="C17">
         <v>33</v>
       </c>
       <c r="E17">
@@ -33668,10 +33725,10 @@
       <c r="A18" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="B18" s="10">
+      <c r="B18">
         <v>929</v>
       </c>
-      <c r="C18" s="10">
+      <c r="C18">
         <v>75</v>
       </c>
       <c r="E18">
@@ -33683,10 +33740,10 @@
       <c r="A19" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="B19" s="10">
+      <c r="B19">
         <v>2576</v>
       </c>
-      <c r="C19" s="10">
+      <c r="C19">
         <v>330</v>
       </c>
       <c r="E19">
@@ -33698,10 +33755,10 @@
       <c r="A20" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="B20" s="10">
+      <c r="B20">
         <v>1033</v>
       </c>
-      <c r="C20" s="10">
+      <c r="C20">
         <v>218</v>
       </c>
       <c r="E20">
@@ -33713,10 +33770,10 @@
       <c r="A21" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="B21" s="10">
+      <c r="B21">
         <v>1020</v>
       </c>
-      <c r="C21" s="10">
+      <c r="C21">
         <v>214</v>
       </c>
       <c r="E21">
@@ -33728,10 +33785,10 @@
       <c r="A22" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="B22" s="10">
+      <c r="B22">
         <v>891</v>
       </c>
-      <c r="C22" s="10">
+      <c r="C22">
         <v>168</v>
       </c>
       <c r="E22">
@@ -33743,10 +33800,10 @@
       <c r="A23" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="B23" s="10">
+      <c r="B23">
         <v>113</v>
       </c>
-      <c r="C23" s="10">
+      <c r="C23">
         <v>33</v>
       </c>
       <c r="E23">
@@ -33758,10 +33815,10 @@
       <c r="A24" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="B24" s="10">
+      <c r="B24">
         <v>16</v>
       </c>
-      <c r="C24" s="10">
+      <c r="C24">
         <v>13</v>
       </c>
       <c r="E24">
@@ -33773,10 +33830,10 @@
       <c r="A25" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="B25" s="10">
+      <c r="B25">
         <v>13</v>
       </c>
-      <c r="C25" s="10">
+      <c r="C25">
         <v>4</v>
       </c>
       <c r="E25">
@@ -33788,10 +33845,10 @@
       <c r="A26" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="B26" s="10">
+      <c r="B26">
         <v>13</v>
       </c>
-      <c r="C26" s="10">
+      <c r="C26">
         <v>4</v>
       </c>
       <c r="E26">
@@ -33803,10 +33860,10 @@
       <c r="A27" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="B27" s="10">
+      <c r="B27">
         <v>6382</v>
       </c>
-      <c r="C27" s="10">
+      <c r="C27">
         <v>792</v>
       </c>
       <c r="E27">
@@ -33821,10 +33878,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C763CAA4-0562-46BE-AE3C-A64DDF4AB21A}">
-  <dimension ref="A1:E21"/>
+  <dimension ref="A1:H27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5:E8"/>
+      <selection activeCell="K23" sqref="K23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -33883,180 +33940,378 @@
       <c r="C5" s="10">
         <v>13</v>
       </c>
-      <c r="D5" t="s">
-        <v>35</v>
-      </c>
       <c r="E5">
-        <f t="shared" ref="E5:E12" si="0">C5/B5*100</f>
+        <f t="shared" ref="E5:E27" si="0">C5/B5*100</f>
         <v>12.871287128712872</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="7" t="s">
-        <v>17</v>
+      <c r="A6" s="9" t="s">
+        <v>20</v>
       </c>
       <c r="B6" s="10">
-        <v>779</v>
+        <v>1</v>
       </c>
       <c r="C6" s="10">
-        <v>62</v>
-      </c>
-      <c r="D6" t="s">
-        <v>37</v>
+        <v>0</v>
       </c>
       <c r="E6">
         <f t="shared" si="0"/>
-        <v>7.9589216944801038</v>
+        <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="7" t="s">
-        <v>18</v>
+      <c r="A7" s="9" t="s">
+        <v>21</v>
       </c>
       <c r="B7" s="10">
-        <v>720</v>
+        <v>100</v>
       </c>
       <c r="C7" s="10">
-        <v>61</v>
-      </c>
-      <c r="D7" t="s">
-        <v>36</v>
+        <v>13</v>
       </c>
       <c r="E7">
         <f t="shared" si="0"/>
-        <v>8.4722222222222232</v>
+        <v>13</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="7" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B8" s="10">
-        <v>3749</v>
+        <v>779</v>
       </c>
       <c r="C8" s="10">
-        <v>438</v>
-      </c>
-      <c r="D8" t="s">
-        <v>38</v>
+        <v>62</v>
       </c>
       <c r="E8">
         <f t="shared" si="0"/>
-        <v>11.683115497465991</v>
+        <v>7.9589216944801038</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" s="6" t="s">
-        <v>13</v>
+      <c r="A9" s="9" t="s">
+        <v>23</v>
       </c>
       <c r="B9" s="10">
-        <v>1033</v>
+        <v>439</v>
       </c>
       <c r="C9" s="10">
-        <v>218</v>
+        <v>41</v>
       </c>
       <c r="E9">
         <f t="shared" si="0"/>
-        <v>21.10358180058083</v>
+        <v>9.3394077448747161</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" s="7" t="s">
-        <v>16</v>
+      <c r="A10" s="9" t="s">
+        <v>24</v>
       </c>
       <c r="B10" s="10">
-        <v>1020</v>
+        <v>113</v>
       </c>
       <c r="C10" s="10">
-        <v>214</v>
-      </c>
-      <c r="D10" t="s">
-        <v>35</v>
+        <v>9</v>
       </c>
       <c r="E10">
         <f t="shared" si="0"/>
-        <v>20.980392156862745</v>
+        <v>7.9646017699115044</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" s="7" t="s">
-        <v>17</v>
+      <c r="A11" s="9" t="s">
+        <v>25</v>
       </c>
       <c r="B11" s="10">
-        <v>13</v>
+        <v>227</v>
       </c>
       <c r="C11" s="10">
-        <v>4</v>
-      </c>
-      <c r="D11" t="s">
-        <v>37</v>
+        <v>12</v>
       </c>
       <c r="E11">
         <f t="shared" si="0"/>
-        <v>30.76923076923077</v>
+        <v>5.286343612334802</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" s="6" t="s">
-        <v>11</v>
+      <c r="A12" s="7" t="s">
+        <v>18</v>
       </c>
       <c r="B12" s="10">
-        <v>6382</v>
+        <v>720</v>
       </c>
       <c r="C12" s="10">
-        <v>792</v>
+        <v>61</v>
       </c>
       <c r="E12">
         <f t="shared" si="0"/>
+        <v>8.4722222222222232</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="B13" s="10">
+        <v>254</v>
+      </c>
+      <c r="C13" s="10">
+        <v>11</v>
+      </c>
+      <c r="E13">
+        <f t="shared" si="0"/>
+        <v>4.3307086614173231</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="B14" s="10">
+        <v>265</v>
+      </c>
+      <c r="C14" s="10">
+        <v>31</v>
+      </c>
+      <c r="E14">
+        <f t="shared" si="0"/>
+        <v>11.69811320754717</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="B15" s="10">
+        <v>201</v>
+      </c>
+      <c r="C15" s="10">
+        <v>19</v>
+      </c>
+      <c r="E15">
+        <f t="shared" si="0"/>
+        <v>9.4527363184079594</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="B16" s="10">
+        <v>3749</v>
+      </c>
+      <c r="C16" s="10">
+        <v>438</v>
+      </c>
+      <c r="E16">
+        <f t="shared" si="0"/>
+        <v>11.683115497465991</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A17" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="B17" s="10">
+        <v>244</v>
+      </c>
+      <c r="C17" s="10">
+        <v>33</v>
+      </c>
+      <c r="E17">
+        <f t="shared" si="0"/>
+        <v>13.524590163934427</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A18" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="B18" s="10">
+        <v>929</v>
+      </c>
+      <c r="C18" s="10">
+        <v>75</v>
+      </c>
+      <c r="E18">
+        <f t="shared" si="0"/>
+        <v>8.0731969860064581</v>
+      </c>
+      <c r="G18" s="8" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A19" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="B19" s="10">
+        <v>2576</v>
+      </c>
+      <c r="C19" s="10">
+        <v>330</v>
+      </c>
+      <c r="E19" s="12">
+        <f t="shared" si="0"/>
+        <v>12.81055900621118</v>
+      </c>
+      <c r="G19" t="s">
+        <v>35</v>
+      </c>
+      <c r="H19">
+        <v>12.871287128712872</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A20" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="B20" s="10">
+        <v>1033</v>
+      </c>
+      <c r="C20" s="10">
+        <v>218</v>
+      </c>
+      <c r="E20">
+        <f t="shared" si="0"/>
+        <v>21.10358180058083</v>
+      </c>
+      <c r="G20" t="s">
+        <v>37</v>
+      </c>
+      <c r="H20">
+        <v>7.9589216944801038</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A21" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="B21" s="10">
+        <v>1020</v>
+      </c>
+      <c r="C21" s="10">
+        <v>214</v>
+      </c>
+      <c r="E21" s="11">
+        <f t="shared" si="0"/>
+        <v>20.980392156862745</v>
+      </c>
+      <c r="G21" t="s">
+        <v>36</v>
+      </c>
+      <c r="H21">
+        <v>8.4722222222222232</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A22" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="B22" s="10">
+        <v>891</v>
+      </c>
+      <c r="C22" s="10">
+        <v>168</v>
+      </c>
+      <c r="E22">
+        <f t="shared" si="0"/>
+        <v>18.855218855218855</v>
+      </c>
+      <c r="G22" t="s">
+        <v>38</v>
+      </c>
+      <c r="H22">
+        <v>11.683115497465991</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A23" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="B23" s="10">
+        <v>113</v>
+      </c>
+      <c r="C23" s="10">
+        <v>33</v>
+      </c>
+      <c r="E23">
+        <f t="shared" si="0"/>
+        <v>29.20353982300885</v>
+      </c>
+      <c r="G23" t="s">
+        <v>39</v>
+      </c>
+      <c r="H23">
+        <v>20.980392156862745</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A24" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="B24" s="10">
+        <v>16</v>
+      </c>
+      <c r="C24" s="10">
+        <v>13</v>
+      </c>
+      <c r="E24">
+        <f t="shared" si="0"/>
+        <v>81.25</v>
+      </c>
+      <c r="G24" t="s">
+        <v>40</v>
+      </c>
+      <c r="H24">
+        <v>30.76923076923077</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A25" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="B25" s="10">
+        <v>13</v>
+      </c>
+      <c r="C25" s="10">
+        <v>4</v>
+      </c>
+      <c r="E25">
+        <f t="shared" si="0"/>
+        <v>30.76923076923077</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A26" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="B26" s="10">
+        <v>13</v>
+      </c>
+      <c r="C26" s="10">
+        <v>4</v>
+      </c>
+      <c r="E26">
+        <f t="shared" si="0"/>
+        <v>30.76923076923077</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A27" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="B27" s="10">
+        <v>6382</v>
+      </c>
+      <c r="C27" s="10">
+        <v>792</v>
+      </c>
+      <c r="E27">
+        <f t="shared" si="0"/>
         <v>12.409902851770605</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>35</v>
-      </c>
-      <c r="B16">
-        <v>12.871287128712872</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>37</v>
-      </c>
-      <c r="B17">
-        <v>7.9589216944801038</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>36</v>
-      </c>
-      <c r="B18">
-        <v>8.4722222222222232</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>38</v>
-      </c>
-      <c r="B19">
-        <v>11.683115497465991</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>39</v>
-      </c>
-      <c r="B20">
-        <v>20.980392156862745</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>40</v>
-      </c>
-      <c r="B21">
-        <v>30.76923076923077</v>
       </c>
     </row>
   </sheetData>

</xml_diff>